<commit_message>
Scheduling and first test
</commit_message>
<xml_diff>
--- a/src/graphs/1rwy-alternating.xlsx
+++ b/src/graphs/1rwy-alternating.xlsx
@@ -10,17 +10,18 @@
     <sheet name="Total delay" sheetId="8" r:id="rId1"/>
     <sheet name="Maximal delay" sheetId="9" r:id="rId2"/>
     <sheet name="Replanned slots" sheetId="11" r:id="rId3"/>
-    <sheet name="List1" sheetId="1" r:id="rId4"/>
-    <sheet name="List2" sheetId="2" r:id="rId5"/>
-    <sheet name="List3" sheetId="3" r:id="rId6"/>
-    <sheet name="List4" sheetId="5" r:id="rId7"/>
+    <sheet name="Makespan" sheetId="12" r:id="rId4"/>
+    <sheet name="List1" sheetId="1" r:id="rId5"/>
+    <sheet name="List2" sheetId="2" r:id="rId6"/>
+    <sheet name="List3" sheetId="3" r:id="rId7"/>
+    <sheet name="List4" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
   <si>
     <t>Slots</t>
   </si>
@@ -95,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +105,26 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,10 +136,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -134,8 +149,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Chybně" xfId="1" builtinId="27"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1424,11 +1442,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109280256"/>
-        <c:axId val="111629440"/>
+        <c:axId val="108682240"/>
+        <c:axId val="110843008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109280256"/>
+        <c:axId val="108682240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1497,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111629440"/>
+        <c:crossAx val="110843008"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1487,7 +1505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111629440"/>
+        <c:axId val="110843008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.5000000000000014E-2"/>
@@ -1533,7 +1551,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109280256"/>
+        <c:crossAx val="108682240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3036,11 +3054,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111707264"/>
-        <c:axId val="111709184"/>
+        <c:axId val="110986368"/>
+        <c:axId val="110988288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111707264"/>
+        <c:axId val="110986368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3095,7 +3113,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111709184"/>
+        <c:crossAx val="110988288"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3103,7 +3121,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111709184"/>
+        <c:axId val="110988288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0000000000000028E-3"/>
@@ -3173,7 +3191,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111707264"/>
+        <c:crossAx val="110986368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4255,11 +4273,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111827584"/>
-        <c:axId val="111878912"/>
+        <c:axId val="111368832"/>
+        <c:axId val="112993024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111827584"/>
+        <c:axId val="111368832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4308,7 +4326,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111878912"/>
+        <c:crossAx val="112993024"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4316,7 +4334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111878912"/>
+        <c:axId val="112993024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="31"/>
@@ -4343,7 +4361,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4362,7 +4379,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111827584"/>
+        <c:crossAx val="111368832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4377,6 +4394,718 @@
           <c:y val="6.8340562380941855E-2"/>
           <c:w val="0.14577146145904843"/>
           <c:h val="0.51391535423290591"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr baseline="0">
+              <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="cs-CZ"/>
+              <a:t>Název</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.42872611614787765"/>
+          <c:y val="3.0563894432451073E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KEEP_ASCENDING</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$L$3:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0810185185185186E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0069444444444441E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7939814814814816E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6689814814814806E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.068287037037037E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1608796296296296E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2395833333333335E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4270833333333335E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6284722222222221E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7210648148148149E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IN_PLACE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$M$3:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7615740740740739E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2013888888888891E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2013888888888891E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5393518518518517E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5393518518518517E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.9791666666666674E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.9791666666666674E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.3171296296296283E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.3171296296296283E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3333333333333332E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AT_THE_END</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$N$3:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.31712962962963E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2430555555555555E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.030092592592593E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.905092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6921296296296312E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.618055555555555E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0405092592592593E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2280092592592592E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.306712962962963E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3993055555555555E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FILL_VOIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$O$3:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.31712962962963E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2430555555555555E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.030092592592593E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.905092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6921296296296312E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.618055555555555E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0405092592592593E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2280092592592592E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.306712962962963E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3993055555555555E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KEEP_ASC_MIN_DELAY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$P$3:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8541666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7800925925925919E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5671296296296302E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4421296296296293E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2291666666666659E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.1550925925925931E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9421296296296289E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1817129629629629E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2604166666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3530092592592594E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MIN_MAKESPAN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$Q$3:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8541666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.076388888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6550925925925935E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4421296296296293E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2291666666666659E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2013888888888892E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.8032407407407408E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0590277777777777E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1377314814814814E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2337962962962962E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MIN_MAX_DELAY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$R$3:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8541666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7800925925925919E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5671296296296302E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4421296296296293E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2291666666666659E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.1550925925925931E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0127314814814815E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2002314814814815E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1562499999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3391203703703704E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MIN_DELAY_SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$S$3:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1921296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.530092592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8541666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7800925925925919E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5671296296296302E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4421296296296293E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4143518518518517E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2013888888888892E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9884259259259266E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0590277777777777E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1377314814814814E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2349537037037039E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="51693824"/>
+        <c:axId val="51863936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="51693824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr baseline="0">
+                    <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Název</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44316013355419237"/>
+              <c:y val="0.91611183977562427"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr baseline="0">
+                <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51863936"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51863936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.7500000000000005E-2"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Název</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr baseline="0">
+                <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51693824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10847083658455971"/>
+          <c:y val="0.11940292077838793"/>
+          <c:w val="0.14577146145904843"/>
+          <c:h val="0.38990676955339393"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4433,6 +5162,17 @@
   <pageMargins left="0" right="0" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
   <pageSetup paperSize="6" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -4495,6 +5235,33 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="7354917" cy="3495495"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graf 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9301307" cy="6003636"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graf 1"/>
@@ -5364,12 +6131,293 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Kancelář">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Kancelář">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Kancelář">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5384,7 +6432,7 @@
     <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
@@ -5399,7 +6447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5419,16 +6467,43 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5456,37 +6531,107 @@
       <c r="I3">
         <v>103000</v>
       </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <f>TIME(INT((B3/1000)/3600),INT(MOD((B3/1000),3600)/60),ROUND(MOD(MOD((B3/1000),3600),60),0))</f>
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="M3" s="2">
+        <f t="shared" ref="M3:S14" si="0">TIME(INT((C3/1000)/3600),INT(MOD((C3/1000),3600)/60),ROUND(MOD(MOD((C3/1000),3600),60),0))</f>
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="N3" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="Q3" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="R3" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1921296296296296E-3</v>
+      </c>
+      <c r="S3" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1921296296296296E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>302425</v>
+        <v>304755</v>
       </c>
       <c r="C4">
-        <v>302425</v>
+        <v>304755</v>
       </c>
       <c r="D4">
-        <v>302425</v>
+        <v>304755</v>
       </c>
       <c r="E4">
-        <v>302425</v>
+        <v>304755</v>
       </c>
       <c r="F4">
-        <v>302425</v>
+        <v>304755</v>
       </c>
       <c r="G4">
-        <v>302425</v>
+        <v>304755</v>
       </c>
       <c r="H4">
-        <v>302425</v>
+        <v>304755</v>
       </c>
       <c r="I4">
-        <v>302425</v>
+        <v>304755</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L14" si="1">TIME(INT((B4/1000)/3600),INT(MOD((B4/1000),3600)/60),ROUND(MOD(MOD((B4/1000),3600),60),0))</f>
+        <v>3.530092592592592E-3</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.530092592592592E-3</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.530092592592592E-3</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.530092592592592E-3</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.530092592592592E-3</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.530092592592592E-3</v>
+      </c>
+      <c r="R4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.530092592592592E-3</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.530092592592592E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5494,13 +6639,13 @@
         <v>439000</v>
       </c>
       <c r="C5">
-        <v>303202</v>
+        <v>325126</v>
       </c>
       <c r="D5">
-        <v>370425</v>
+        <v>372755</v>
       </c>
       <c r="E5">
-        <v>370425</v>
+        <v>372755</v>
       </c>
       <c r="F5">
         <v>333000</v>
@@ -5514,37 +6659,107 @@
       <c r="I5">
         <v>333000</v>
       </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0810185185185186E-3</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7615740740740739E-3</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>4.31712962962963E-3</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="0"/>
+        <v>4.31712962962963E-3</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8541666666666668E-3</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8541666666666668E-3</v>
+      </c>
+      <c r="R5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8541666666666668E-3</v>
+      </c>
+      <c r="S5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8541666666666668E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <v>519000</v>
       </c>
-      <c r="C6">
-        <v>343777</v>
+      <c r="C6" s="4">
+        <v>363371</v>
       </c>
       <c r="D6">
-        <v>450425</v>
+        <v>452755</v>
       </c>
       <c r="E6">
-        <v>450425</v>
+        <v>452755</v>
       </c>
       <c r="F6">
         <v>413000</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
+        <v>525371</v>
+      </c>
+      <c r="H6">
         <v>413000</v>
-      </c>
-      <c r="H6">
-        <v>507000</v>
       </c>
       <c r="I6">
         <v>413000</v>
       </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="1"/>
+        <v>6.0069444444444441E-3</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2013888888888891E-3</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2430555555555555E-3</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2430555555555555E-3</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7800925925925919E-3</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="0"/>
+        <v>6.076388888888889E-3</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7800925925925919E-3</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7800925925925919E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5552,28 +6767,63 @@
         <v>587000</v>
       </c>
       <c r="C7">
-        <v>343777</v>
+        <v>363371</v>
       </c>
       <c r="D7">
-        <v>518425</v>
+        <v>520755</v>
       </c>
       <c r="E7">
-        <v>518425</v>
+        <v>520755</v>
       </c>
       <c r="F7">
         <v>481000</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
+        <v>575000</v>
+      </c>
+      <c r="H7">
         <v>481000</v>
-      </c>
-      <c r="H7">
-        <v>573000</v>
       </c>
       <c r="I7">
         <v>481000</v>
       </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="1"/>
+        <v>6.7939814814814816E-3</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2013888888888891E-3</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.030092592592593E-3</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.030092592592593E-3</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5671296296296302E-3</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.6550925925925935E-3</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5671296296296302E-3</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5671296296296302E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5581,13 +6831,13 @@
         <v>749000</v>
       </c>
       <c r="C8">
-        <v>543202</v>
+        <v>565126</v>
       </c>
       <c r="D8">
-        <v>680425</v>
+        <v>682755</v>
       </c>
       <c r="E8">
-        <v>680425</v>
+        <v>682755</v>
       </c>
       <c r="F8">
         <v>643000</v>
@@ -5596,13 +6846,48 @@
         <v>643000</v>
       </c>
       <c r="H8">
-        <v>641000</v>
+        <v>643000</v>
       </c>
       <c r="I8">
         <v>643000</v>
       </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6689814814814806E-3</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="0"/>
+        <v>6.5393518518518517E-3</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4421296296296293E-3</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4421296296296293E-3</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4421296296296293E-3</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4421296296296293E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5610,28 +6895,63 @@
         <v>923000</v>
       </c>
       <c r="C9">
-        <v>543202</v>
+        <v>565126</v>
       </c>
       <c r="D9">
-        <v>748425</v>
+        <v>750755</v>
       </c>
       <c r="E9">
-        <v>748425</v>
+        <v>750755</v>
       </c>
       <c r="F9">
         <v>711000</v>
       </c>
       <c r="G9">
-        <v>709000</v>
+        <v>711000</v>
       </c>
       <c r="H9">
         <v>711000</v>
       </c>
       <c r="I9">
-        <v>711000</v>
+        <v>726629</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.068287037037037E-2</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="0"/>
+        <v>6.5393518518518517E-3</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.6921296296296312E-3</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.6921296296296312E-3</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2291666666666659E-3</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2291666666666659E-3</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2291666666666659E-3</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.4143518518518517E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5639,28 +6959,63 @@
         <v>1003000</v>
       </c>
       <c r="C10">
-        <v>583777</v>
+        <v>603371</v>
       </c>
       <c r="D10">
-        <v>828425</v>
+        <v>830755</v>
       </c>
       <c r="E10">
-        <v>828425</v>
+        <v>830755</v>
       </c>
       <c r="F10">
         <v>791000</v>
       </c>
       <c r="G10">
+        <v>794629</v>
+      </c>
+      <c r="H10">
         <v>791000</v>
       </c>
-      <c r="H10">
-        <v>813000</v>
-      </c>
       <c r="I10">
-        <v>814223</v>
+        <v>794629</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1608796296296296E-2</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9791666666666674E-3</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.618055555555555E-3</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.618055555555555E-3</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.1550925925925931E-3</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.2013888888888892E-3</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.1550925925925931E-3</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.2013888888888892E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5668,28 +7023,63 @@
         <v>1071000</v>
       </c>
       <c r="C11">
-        <v>583777</v>
+        <v>603371</v>
       </c>
       <c r="D11">
-        <v>896425</v>
+        <v>898755</v>
       </c>
       <c r="E11">
-        <v>896425</v>
+        <v>898755</v>
       </c>
       <c r="F11">
         <v>859000</v>
       </c>
       <c r="G11">
-        <v>859000</v>
+        <v>847000</v>
       </c>
       <c r="H11">
-        <v>847000</v>
+        <v>874629</v>
       </c>
       <c r="I11">
-        <v>847000</v>
+        <v>862629</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2395833333333335E-2</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9791666666666674E-3</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0405092592592593E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0405092592592593E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9421296296296289E-3</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8032407407407408E-3</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0127314814814815E-2</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9884259259259266E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5697,86 +7087,191 @@
         <v>1233000</v>
       </c>
       <c r="C12">
-        <v>783201</v>
+        <v>805126</v>
       </c>
       <c r="D12">
-        <v>1058425</v>
+        <v>1060755</v>
       </c>
       <c r="E12">
-        <v>1058425</v>
+        <v>1060755</v>
       </c>
       <c r="F12">
         <v>1021000</v>
       </c>
       <c r="G12">
-        <v>1021000</v>
-      </c>
-      <c r="H12">
         <v>915000</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1036629</v>
       </c>
       <c r="I12">
         <v>915000</v>
       </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4270833333333335E-2</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3171296296296283E-3</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2280092592592592E-2</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2280092592592592E-2</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1817129629629629E-2</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0590277777777777E-2</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2002314814814815E-2</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0590277777777777E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <v>1407000</v>
       </c>
-      <c r="C13">
-        <v>783201</v>
+      <c r="C13" s="5">
+        <v>805126</v>
       </c>
       <c r="D13">
-        <v>1126425</v>
+        <v>1128755</v>
       </c>
       <c r="E13">
-        <v>1126425</v>
+        <v>1128755</v>
       </c>
       <c r="F13">
         <v>1089000</v>
       </c>
       <c r="G13">
-        <v>1018223</v>
-      </c>
-      <c r="H13">
         <v>983000</v>
+      </c>
+      <c r="H13" s="5">
+        <v>998629</v>
       </c>
       <c r="I13">
         <v>983000</v>
       </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6284722222222221E-2</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3171296296296283E-3</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.306712962962963E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.306712962962963E-2</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2604166666666666E-2</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1377314814814814E-2</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1562499999999998E-2</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1377314814814814E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <v>1487000</v>
       </c>
-      <c r="C14">
-        <v>723555</v>
+      <c r="C14" s="5">
+        <v>720050</v>
       </c>
       <c r="D14">
-        <v>1206425</v>
+        <v>1208755</v>
       </c>
       <c r="E14">
-        <v>1206425</v>
+        <v>1208755</v>
       </c>
       <c r="F14">
         <v>1169000</v>
       </c>
       <c r="G14">
-        <v>1063000</v>
+        <v>1065679</v>
       </c>
       <c r="H14">
-        <v>1086223</v>
+        <v>1157000</v>
       </c>
       <c r="I14">
-        <v>1063000</v>
+        <v>1066629</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7210648148148149E-2</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3993055555555555E-2</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3993055555555555E-2</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3530092592592594E-2</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2337962962962962E-2</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3391203703703704E-2</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2349537037037039E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -5880,31 +7375,31 @@
         <v>0</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" ref="M18:S29" si="0">TIME(INT((C18/1000)/3600),INT(MOD((C18/1000),3600)/60),ROUND(MOD(MOD((C18/1000),3600),60),0))</f>
+        <f t="shared" ref="M18:S29" si="2">TIME(INT((C18/1000)/3600),INT(MOD((C18/1000),3600)/60),ROUND(MOD(MOD((C18/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5940,35 +7435,35 @@
         <v>2</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" ref="L19:L29" si="1">TIME(INT((B19/1000)/3600),INT(MOD((B19/1000),3600)/60),ROUND(MOD(MOD((B19/1000),3600),60),0))</f>
+        <f t="shared" ref="L19:L29" si="3">TIME(INT((B19/1000)/3600),INT(MOD((B19/1000),3600)/60),ROUND(MOD(MOD((B19/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6004,35 +7499,35 @@
         <v>3</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0138888888888888E-3</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0138888888888888E-3</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0023148148148148E-3</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.9861111111111105E-4</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.9861111111111105E-4</v>
       </c>
       <c r="R20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.9861111111111105E-4</v>
       </c>
       <c r="S20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.9861111111111105E-4</v>
       </c>
     </row>
@@ -6068,35 +7563,35 @@
         <v>4</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0138888888888888E-3</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0138888888888888E-3</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0254629629629629E-3</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1018518518518516E-4</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3611111111111111E-3</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1018518518518516E-4</v>
       </c>
       <c r="S21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1018518518518516E-4</v>
       </c>
     </row>
@@ -6132,35 +7627,35 @@
         <v>5</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1944444444444442E-3</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1944444444444442E-3</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1828703703703702E-3</v>
       </c>
       <c r="P22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9675925925925928E-3</v>
       </c>
       <c r="Q22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.363425925925926E-3</v>
       </c>
       <c r="R22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9675925925925928E-3</v>
       </c>
       <c r="S22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7546296296296294E-3</v>
       </c>
     </row>
@@ -6196,35 +7691,35 @@
         <v>6</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1944444444444442E-3</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1944444444444442E-3</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1828703703703702E-3</v>
       </c>
       <c r="P23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9675925925925928E-3</v>
       </c>
       <c r="Q23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.1504629629629635E-3</v>
       </c>
       <c r="R23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9675925925925928E-3</v>
       </c>
       <c r="S23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7546296296296294E-3</v>
       </c>
     </row>
@@ -6260,35 +7755,35 @@
         <v>7</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6111111111111114E-3</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6111111111111114E-3</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.8263888888888887E-3</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3958333333333336E-3</v>
       </c>
       <c r="Q24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.9375000000000009E-3</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3958333333333336E-3</v>
       </c>
       <c r="S24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1828703703703702E-3</v>
       </c>
     </row>
@@ -6324,35 +7819,35 @@
         <v>8</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6111111111111114E-3</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6111111111111114E-3</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.8495370370370368E-3</v>
       </c>
       <c r="P25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4074074074074076E-3</v>
       </c>
       <c r="Q25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.363425925925926E-3</v>
       </c>
       <c r="R25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4074074074074076E-3</v>
       </c>
       <c r="S25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.7337962962962958E-3</v>
       </c>
     </row>
@@ -6388,35 +7883,35 @@
         <v>9</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.7916666666666672E-3</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.7916666666666672E-3</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0069444444444441E-3</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.5648148148148154E-3</v>
       </c>
       <c r="Q26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.7569444444444447E-3</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1944444444444442E-3</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.7569444444444447E-3</v>
       </c>
     </row>
@@ -6452,35 +7947,35 @@
         <v>10</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.7916666666666672E-3</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.7916666666666672E-3</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0069444444444441E-3</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.5648148148148154E-3</v>
       </c>
       <c r="Q27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.5439814814814822E-3</v>
       </c>
       <c r="R27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1944444444444442E-3</v>
       </c>
       <c r="S27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.5439814814814822E-3</v>
       </c>
     </row>
@@ -6516,35 +8011,35 @@
         <v>11</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.6504629629629631E-3</v>
       </c>
       <c r="P28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.9930555555555561E-3</v>
       </c>
       <c r="Q28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.3310185185185197E-3</v>
       </c>
       <c r="R28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.9351851851851857E-3</v>
       </c>
       <c r="S28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.3310185185185197E-3</v>
       </c>
     </row>
@@ -6580,35 +8075,35 @@
         <v>12</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.6018518518518518E-3</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.6018518518518518E-3</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.8310185185185176E-3</v>
       </c>
       <c r="P29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.162037037037037E-3</v>
       </c>
       <c r="Q29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.2962962962962964E-3</v>
       </c>
       <c r="R29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.9699074074074072E-3</v>
       </c>
       <c r="S29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.3310185185185197E-3</v>
       </c>
     </row>
@@ -6712,35 +8207,35 @@
         <v>1</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" ref="L33:L44" si="2">TIME(INT((B33/1000)/3600),INT(MOD((B33/1000),3600)/60),ROUND(MOD(MOD((B33/1000),3600),60),0))</f>
+        <f t="shared" ref="L33:L44" si="4">TIME(INT((B33/1000)/3600),INT(MOD((B33/1000),3600)/60),ROUND(MOD(MOD((B33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33:M44" si="3">TIME(INT((C33/1000)/3600),INT(MOD((C33/1000),3600)/60),ROUND(MOD(MOD((C33/1000),3600),60),0))</f>
+        <f t="shared" ref="M33:M44" si="5">TIME(INT((C33/1000)/3600),INT(MOD((C33/1000),3600)/60),ROUND(MOD(MOD((C33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" ref="N33:N44" si="4">TIME(INT((D33/1000)/3600),INT(MOD((D33/1000),3600)/60),ROUND(MOD(MOD((D33/1000),3600),60),0))</f>
+        <f t="shared" ref="N33:N44" si="6">TIME(INT((D33/1000)/3600),INT(MOD((D33/1000),3600)/60),ROUND(MOD(MOD((D33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="O33" s="2">
-        <f t="shared" ref="O33:O44" si="5">TIME(INT((E33/1000)/3600),INT(MOD((E33/1000),3600)/60),ROUND(MOD(MOD((E33/1000),3600),60),0))</f>
+        <f t="shared" ref="O33:O44" si="7">TIME(INT((E33/1000)/3600),INT(MOD((E33/1000),3600)/60),ROUND(MOD(MOD((E33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="P33" s="2">
-        <f t="shared" ref="P33:P44" si="6">TIME(INT((F33/1000)/3600),INT(MOD((F33/1000),3600)/60),ROUND(MOD(MOD((F33/1000),3600),60),0))</f>
+        <f t="shared" ref="P33:P44" si="8">TIME(INT((F33/1000)/3600),INT(MOD((F33/1000),3600)/60),ROUND(MOD(MOD((F33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="Q33" s="2">
-        <f t="shared" ref="Q33:Q44" si="7">TIME(INT((G33/1000)/3600),INT(MOD((G33/1000),3600)/60),ROUND(MOD(MOD((G33/1000),3600),60),0))</f>
+        <f t="shared" ref="Q33:Q44" si="9">TIME(INT((G33/1000)/3600),INT(MOD((G33/1000),3600)/60),ROUND(MOD(MOD((G33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="R33" s="2">
-        <f t="shared" ref="R33:R44" si="8">TIME(INT((H33/1000)/3600),INT(MOD((H33/1000),3600)/60),ROUND(MOD(MOD((H33/1000),3600),60),0))</f>
+        <f t="shared" ref="R33:R44" si="10">TIME(INT((H33/1000)/3600),INT(MOD((H33/1000),3600)/60),ROUND(MOD(MOD((H33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="S33" s="2">
-        <f t="shared" ref="S33:S44" si="9">TIME(INT((I33/1000)/3600),INT(MOD((I33/1000),3600)/60),ROUND(MOD(MOD((I33/1000),3600),60),0))</f>
+        <f t="shared" ref="S33:S44" si="11">TIME(INT((I33/1000)/3600),INT(MOD((I33/1000),3600)/60),ROUND(MOD(MOD((I33/1000),3600),60),0))</f>
         <v>0</v>
       </c>
       <c r="T33" s="2"/>
@@ -6778,35 +8273,35 @@
         <v>2</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q34" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R34" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S34" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T34" s="2"/>
@@ -6844,35 +8339,35 @@
         <v>3</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.0138888888888888E-3</v>
       </c>
       <c r="N35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.0138888888888888E-3</v>
       </c>
       <c r="O35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.5763888888888894E-3</v>
       </c>
       <c r="P35" s="2">
-        <f t="shared" si="6"/>
-        <v>1.1458333333333333E-3</v>
-      </c>
-      <c r="Q35" s="2">
-        <f t="shared" si="7"/>
-        <v>1.1458333333333333E-3</v>
-      </c>
-      <c r="R35" s="2">
         <f t="shared" si="8"/>
         <v>1.1458333333333333E-3</v>
       </c>
+      <c r="Q35" s="2">
+        <f t="shared" si="9"/>
+        <v>1.1458333333333333E-3</v>
+      </c>
+      <c r="R35" s="2">
+        <f t="shared" si="10"/>
+        <v>1.1458333333333333E-3</v>
+      </c>
       <c r="S35" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.1458333333333333E-3</v>
       </c>
       <c r="T35" s="2"/>
@@ -6910,35 +8405,35 @@
         <v>4</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.2638888888888891E-3</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.2638888888888891E-3</v>
       </c>
       <c r="O36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.6018518518518518E-3</v>
       </c>
       <c r="P36" s="2">
-        <f t="shared" si="6"/>
-        <v>1.9560185185185184E-3</v>
-      </c>
-      <c r="Q36" s="2">
-        <f t="shared" si="7"/>
-        <v>4.3749999999999995E-3</v>
-      </c>
-      <c r="R36" s="2">
         <f t="shared" si="8"/>
         <v>1.9560185185185184E-3</v>
       </c>
+      <c r="Q36" s="2">
+        <f t="shared" si="9"/>
+        <v>4.3749999999999995E-3</v>
+      </c>
+      <c r="R36" s="2">
+        <f t="shared" si="10"/>
+        <v>1.9560185185185184E-3</v>
+      </c>
       <c r="S36" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.9560185185185184E-3</v>
       </c>
       <c r="T36" s="2"/>
@@ -6976,35 +8471,35 @@
         <v>5</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.4467592592592597E-3</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.4467592592592597E-3</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.5833333333333343E-3</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="6"/>
-        <v>4.7222222222222223E-3</v>
-      </c>
-      <c r="Q37" s="2">
-        <f t="shared" si="7"/>
-        <v>6.7013888888888887E-3</v>
-      </c>
-      <c r="R37" s="2">
         <f t="shared" si="8"/>
         <v>4.7222222222222223E-3</v>
       </c>
+      <c r="Q37" s="2">
+        <f t="shared" si="9"/>
+        <v>6.7013888888888887E-3</v>
+      </c>
+      <c r="R37" s="2">
+        <f t="shared" si="10"/>
+        <v>4.7222222222222223E-3</v>
+      </c>
       <c r="S37" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4.7222222222222223E-3</v>
       </c>
       <c r="T37" s="2"/>
@@ -7042,35 +8537,35 @@
         <v>6</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.0439814814814818E-3</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.0439814814814818E-3</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.1956018518518517E-2</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="6"/>
-        <v>5.8796296296296296E-3</v>
-      </c>
-      <c r="Q38" s="2">
-        <f t="shared" si="7"/>
-        <v>7.8472222222222224E-3</v>
-      </c>
-      <c r="R38" s="2">
         <f t="shared" si="8"/>
         <v>5.8796296296296296E-3</v>
       </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="9"/>
+        <v>7.8472222222222224E-3</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="10"/>
+        <v>5.8796296296296296E-3</v>
+      </c>
       <c r="S38" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5.8796296296296296E-3</v>
       </c>
       <c r="T38" s="2"/>
@@ -7108,35 +8603,35 @@
         <v>7</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1655092592592594E-2</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1655092592592594E-2</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.8807870370370371E-2</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="6"/>
-        <v>9.0624999999999994E-3</v>
-      </c>
-      <c r="Q39" s="2">
-        <f t="shared" si="7"/>
-        <v>1.1006944444444444E-2</v>
-      </c>
-      <c r="R39" s="2">
         <f t="shared" si="8"/>
         <v>9.0624999999999994E-3</v>
       </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="9"/>
+        <v>1.1006944444444444E-2</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="10"/>
+        <v>9.0624999999999994E-3</v>
+      </c>
       <c r="S39" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9.0624999999999994E-3</v>
       </c>
       <c r="T39" s="2"/>
@@ -7174,35 +8669,35 @@
         <v>8</v>
       </c>
       <c r="L40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.4502314814814815E-2</v>
       </c>
       <c r="N40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.4502314814814815E-2</v>
       </c>
       <c r="O40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.3668981481481485E-2</v>
       </c>
       <c r="P40" s="2">
-        <f t="shared" si="6"/>
-        <v>1.1469907407407408E-2</v>
-      </c>
-      <c r="Q40" s="2">
-        <f t="shared" si="7"/>
-        <v>1.1423611111111112E-2</v>
-      </c>
-      <c r="R40" s="2">
         <f t="shared" si="8"/>
         <v>1.1469907407407408E-2</v>
       </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="9"/>
+        <v>1.1423611111111112E-2</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="10"/>
+        <v>1.1469907407407408E-2</v>
+      </c>
       <c r="S40" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.105324074074074E-2</v>
       </c>
       <c r="T40" s="2"/>
@@ -7240,35 +8735,35 @@
         <v>9</v>
       </c>
       <c r="L41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.9293981481481485E-2</v>
       </c>
       <c r="N41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9293981481481485E-2</v>
       </c>
       <c r="O41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.0462962962962966E-2</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.5821759259259261E-2</v>
       </c>
       <c r="Q41" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.3368055555555557E-2</v>
       </c>
       <c r="R41" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.4594907407407405E-2</v>
       </c>
       <c r="S41" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.3368055555555557E-2</v>
       </c>
       <c r="T41" s="2"/>
@@ -7306,35 +8801,35 @@
         <v>10</v>
       </c>
       <c r="L42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.2488425925925926E-2</v>
       </c>
       <c r="N42" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.2488425925925926E-2</v>
       </c>
       <c r="O42" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.5671296296296298E-2</v>
       </c>
       <c r="P42" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.8587962962962962E-2</v>
       </c>
       <c r="Q42" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.4907407407407406E-2</v>
       </c>
       <c r="R42" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="S42" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.4907407407407406E-2</v>
       </c>
       <c r="T42" s="2"/>
@@ -7372,35 +8867,35 @@
         <v>11</v>
       </c>
       <c r="L43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.7696759259259258E-2</v>
       </c>
       <c r="N43" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.7696759259259258E-2</v>
       </c>
       <c r="O43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.5347222222222226E-2</v>
       </c>
       <c r="P43" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.3368055555555555E-2</v>
       </c>
       <c r="Q43" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.8460648148148146E-2</v>
       </c>
       <c r="R43" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.0486111111111111E-2</v>
       </c>
       <c r="S43" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.8460648148148146E-2</v>
       </c>
       <c r="T43" s="2"/>
@@ -7438,35 +8933,35 @@
         <v>12</v>
       </c>
       <c r="L44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.3287037037037039E-2</v>
       </c>
       <c r="N44" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3287037037037039E-2</v>
       </c>
       <c r="O44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.4178240740740735E-2</v>
       </c>
       <c r="P44" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.8530092592592593E-2</v>
       </c>
       <c r="Q44" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.361111111111111E-2</v>
       </c>
       <c r="R44" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.2395833333333334E-2</v>
       </c>
       <c r="S44" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.2395833333333334E-2</v>
       </c>
       <c r="T44" s="2"/>
@@ -7576,31 +9071,31 @@
         <v>0</v>
       </c>
       <c r="M48">
-        <f t="shared" ref="M48:S48" si="10">C48</f>
+        <f t="shared" ref="M48:S48" si="12">C48</f>
         <v>0</v>
       </c>
       <c r="N48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7640,31 +9135,31 @@
         <v>0</v>
       </c>
       <c r="M49">
-        <f t="shared" ref="M49:S49" si="11">M48+C49</f>
+        <f t="shared" ref="M49:S49" si="13">M48+C49</f>
         <v>0</v>
       </c>
       <c r="N49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="S49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -7700,35 +9195,35 @@
         <v>3</v>
       </c>
       <c r="L50">
-        <f t="shared" ref="L50:L59" si="12">L49+B50</f>
+        <f t="shared" ref="L50:L59" si="14">L49+B50</f>
         <v>0</v>
       </c>
       <c r="M50">
-        <f t="shared" ref="M50:M59" si="13">M49+C50</f>
+        <f t="shared" ref="M50:M59" si="15">M49+C50</f>
         <v>0</v>
       </c>
       <c r="N50">
-        <f t="shared" ref="N50:N59" si="14">N49+D50</f>
+        <f t="shared" ref="N50:N59" si="16">N49+D50</f>
         <v>0</v>
       </c>
       <c r="O50">
-        <f t="shared" ref="O50:O59" si="15">O49+E50</f>
+        <f t="shared" ref="O50:O59" si="17">O49+E50</f>
         <v>2</v>
       </c>
       <c r="P50">
-        <f t="shared" ref="P50:P59" si="16">P49+F50</f>
+        <f t="shared" ref="P50:P59" si="18">P49+F50</f>
         <v>1</v>
       </c>
       <c r="Q50">
-        <f t="shared" ref="Q50:Q59" si="17">Q49+G50</f>
+        <f t="shared" ref="Q50:Q59" si="19">Q49+G50</f>
         <v>1</v>
       </c>
       <c r="R50">
-        <f t="shared" ref="R50:R59" si="18">R49+H50</f>
+        <f t="shared" ref="R50:R59" si="20">R49+H50</f>
         <v>1</v>
       </c>
       <c r="S50">
-        <f t="shared" ref="S50:S59" si="19">S49+I50</f>
+        <f t="shared" ref="S50:S59" si="21">S49+I50</f>
         <v>1</v>
       </c>
     </row>
@@ -7764,35 +9259,35 @@
         <v>4</v>
       </c>
       <c r="L51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O51">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="P51">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="Q51">
-        <f t="shared" si="17"/>
-        <v>4</v>
-      </c>
-      <c r="R51">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
+      <c r="Q51">
+        <f t="shared" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
       <c r="S51">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
@@ -7828,35 +9323,35 @@
         <v>5</v>
       </c>
       <c r="L52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="P52">
-        <f t="shared" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="Q52">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="R52">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
+      <c r="Q52">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
       <c r="S52">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
@@ -7892,35 +9387,35 @@
         <v>6</v>
       </c>
       <c r="L53">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O53">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="P53">
-        <f t="shared" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="Q53">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="R53">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
+      <c r="Q53">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
       <c r="S53">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
@@ -7956,35 +9451,35 @@
         <v>7</v>
       </c>
       <c r="L54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M54">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P54">
-        <f t="shared" si="16"/>
-        <v>3</v>
-      </c>
-      <c r="Q54">
-        <f t="shared" si="17"/>
-        <v>11</v>
-      </c>
-      <c r="R54">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
+      <c r="Q54">
+        <f t="shared" si="19"/>
+        <v>11</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
       <c r="S54">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
@@ -8020,35 +9515,35 @@
         <v>8</v>
       </c>
       <c r="L55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N55">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P55">
-        <f t="shared" si="16"/>
-        <v>3</v>
-      </c>
-      <c r="Q55">
-        <f t="shared" si="17"/>
-        <v>17</v>
-      </c>
-      <c r="R55">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
+      <c r="Q55">
+        <f t="shared" si="19"/>
+        <v>17</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
       <c r="S55">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5</v>
       </c>
     </row>
@@ -8084,35 +9579,35 @@
         <v>9</v>
       </c>
       <c r="L56">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M56">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N56">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="P56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>20</v>
       </c>
       <c r="R56">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="S56">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
     </row>
@@ -8148,35 +9643,35 @@
         <v>10</v>
       </c>
       <c r="L57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O57">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="P57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>21</v>
       </c>
       <c r="R57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="S57">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -8212,35 +9707,35 @@
         <v>11</v>
       </c>
       <c r="L58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O58">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="P58">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
       <c r="R58">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="S58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>13</v>
       </c>
     </row>
@@ -8276,35 +9771,35 @@
         <v>12</v>
       </c>
       <c r="L59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="P59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>31</v>
       </c>
       <c r="R59">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>23</v>
       </c>
       <c r="S59">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>13</v>
       </c>
     </row>

</xml_diff>